<commit_message>
comiiting changes to code and data
</commit_message>
<xml_diff>
--- a/CFU_Test_Data.xlsx
+++ b/CFU_Test_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/rstor-henao_lab/Pablo/CFU pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/rstor-henao_lab/Pablo/CFU_Pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77920091-0742-0E4B-B1B3-EFF146305CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D1EE65-4213-8549-AB3C-4C7454530A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25720" yWindow="0" windowWidth="25480" windowHeight="28800" activeTab="1" xr2:uid="{1BBA8D1C-B972-0C41-ACCB-38D29157F936}"/>
+    <workbookView xWindow="25720" yWindow="500" windowWidth="25480" windowHeight="28300" activeTab="1" xr2:uid="{1BBA8D1C-B972-0C41-ACCB-38D29157F936}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="30">
   <si>
     <t>count_date</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>volume_plated_ml</t>
+  </si>
+  <si>
+    <t>dil_4</t>
+  </si>
+  <si>
+    <t>dil_5</t>
+  </si>
+  <si>
+    <t>dil_6</t>
+  </si>
+  <si>
+    <t>dil_7</t>
+  </si>
+  <si>
+    <t>dil_8</t>
   </si>
 </sst>
 </file>
@@ -535,10 +550,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E650AE8-407E-D946-9C61-A0F3494F6485}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,7 +562,7 @@
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,8 +593,23 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -610,8 +640,23 @@
       <c r="J2" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -642,8 +687,23 @@
       <c r="J3" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -674,8 +734,23 @@
       <c r="J4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -706,8 +781,23 @@
       <c r="J5" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -738,8 +828,23 @@
       <c r="J6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -770,8 +875,23 @@
       <c r="J7" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -802,8 +922,23 @@
       <c r="J8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -834,8 +969,23 @@
       <c r="J9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -866,8 +1016,23 @@
       <c r="J10" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -898,8 +1063,23 @@
       <c r="J11" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -930,8 +1110,23 @@
       <c r="J12" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -962,8 +1157,23 @@
       <c r="J13" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -994,8 +1204,23 @@
       <c r="J14" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1026,8 +1251,23 @@
       <c r="J15" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1058,8 +1298,23 @@
       <c r="J16" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1090,8 +1345,23 @@
       <c r="J17" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1122,8 +1392,23 @@
       <c r="J18" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1154,8 +1439,23 @@
       <c r="J19" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1186,8 +1486,23 @@
       <c r="J20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1218,8 +1533,23 @@
       <c r="J21" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1250,8 +1580,23 @@
       <c r="J22" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1282,8 +1627,23 @@
       <c r="J23" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1314,8 +1674,23 @@
       <c r="J24" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1346,8 +1721,23 @@
       <c r="J25" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1378,8 +1768,23 @@
       <c r="J26" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1410,8 +1815,23 @@
       <c r="J27" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1442,8 +1862,23 @@
       <c r="J28" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1474,8 +1909,23 @@
       <c r="J29" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1506,8 +1956,23 @@
       <c r="J30" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -1537,6 +2002,21 @@
       </c>
       <c r="J31" s="1">
         <v>115</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>